<commit_message>
updated sprint-backlog for sprint 5/6
</commit_message>
<xml_diff>
--- a/sprint-backlog/sprint-5/report-sheet.xlsx
+++ b/sprint-backlog/sprint-5/report-sheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="plan" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="30">
   <si>
     <t xml:space="preserve">User Story</t>
   </si>
@@ -97,6 +97,12 @@
   </si>
   <si>
     <t xml:space="preserve">T33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J:2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K:6</t>
   </si>
   <si>
     <t xml:space="preserve">day</t>
@@ -279,7 +285,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -466,11 +472,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="28884390"/>
-        <c:axId val="11396369"/>
+        <c:axId val="6885217"/>
+        <c:axId val="7637786"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="28884390"/>
+        <c:axId val="6885217"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -506,14 +512,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="11396369"/>
+        <c:crossAx val="7637786"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="11396369"/>
+        <c:axId val="7637786"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -556,7 +562,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="28884390"/>
+        <c:crossAx val="6885217"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -605,9 +611,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>47160</xdr:colOff>
+      <xdr:colOff>46800</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>153000</xdr:rowOff>
+      <xdr:rowOff>152640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -615,8 +621,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2733840" y="1339560"/>
-        <a:ext cx="9505080" cy="4127040"/>
+        <a:off x="2733840" y="1348560"/>
+        <a:ext cx="9504720" cy="4126320"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -837,8 +843,8 @@
   </sheetPr>
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H21" activeCellId="0" sqref="H21"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -910,6 +916,12 @@
       <c r="D4" s="0" t="n">
         <v>6</v>
       </c>
+      <c r="H4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
@@ -921,6 +933,9 @@
       <c r="D5" s="0" t="n">
         <v>6</v>
       </c>
+      <c r="I5" s="0" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
@@ -945,6 +960,12 @@
       </c>
       <c r="D7" s="0" t="n">
         <v>8</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -979,7 +1000,7 @@
   </sheetPr>
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
     </sheetView>
   </sheetViews>
@@ -990,7 +1011,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B1" s="0" t="n">
         <v>0</v>
@@ -1013,7 +1034,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>28</v>
@@ -1036,7 +1057,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>28</v>

</xml_diff>

<commit_message>
Added sprint 05 files
</commit_message>
<xml_diff>
--- a/sprint-backlog/sprint-5/report-sheet.xlsx
+++ b/sprint-backlog/sprint-5/report-sheet.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeffc\Git\Team14\sprint-backlog\sprint-5\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C827F58-F21B-4B81-B09F-21C552E29A39}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="986" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="986" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="plan" sheetId="1" r:id="rId1"/>
@@ -120,7 +126,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -161,7 +167,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -233,12 +239,30 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="zh-CN"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -260,7 +284,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1400" b="0" strike="noStrike" spc="-1">
+              <a:rPr lang="en-CA" sz="1400" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -271,17 +295,19 @@
                 </a:uFill>
                 <a:latin typeface="Calibri"/>
               </a:rPr>
-              <a:t>Sprint 4: Burndown Chart Provisional vs Actual</a:t>
+              <a:t>Sprint 5: Burndown Chart Provisional vs Actual</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -301,6 +327,7 @@
               <a:solidFill>
                 <a:srgbClr val="636363"/>
               </a:solidFill>
+              <a:prstDash val="dash"/>
               <a:round/>
             </a:ln>
           </c:spPr>
@@ -334,6 +361,12 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E84B-4F83-A01D-E0A32A08A63F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -387,7 +420,21 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E84B-4F83-A01D-E0A32A08A63F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:hiLowLines>
           <c:spPr>
             <a:ln>
@@ -395,7 +442,7 @@
             </a:ln>
           </c:spPr>
         </c:hiLowLines>
-        <c:marker val="1"/>
+        <c:smooth val="0"/>
         <c:axId val="170134528"/>
         <c:axId val="170148608"/>
       </c:lineChart>
@@ -404,9 +451,11 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:ln w="9360">
@@ -433,7 +482,7 @@
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="170148608"/>
@@ -441,12 +490,14 @@
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="170148608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -460,6 +511,7 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:ln w="6480">
@@ -483,7 +535,7 @@
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="170134528"/>
@@ -499,7 +551,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -513,12 +565,13 @@
           <a:pPr>
             <a:defRPr lang="en-US"/>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -556,7 +609,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -575,7 +634,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -617,7 +676,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -649,9 +708,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -683,6 +760,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -858,18 +953,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="6" width="8.5546875"/>
-    <col min="7" max="7" width="10.44140625"/>
-    <col min="8" max="1025" width="8.5546875"/>
+    <col min="1" max="6" width="8.54296875"/>
+    <col min="7" max="7" width="10.453125"/>
+    <col min="8" max="1025" width="8.54296875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -1043,16 +1138,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1025" width="8.5546875"/>
+    <col min="1" max="1025" width="8.54296875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -1208,16 +1303,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1025" width="8.5546875"/>
+    <col min="1" max="1025" width="8.54296875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">

</xml_diff>